<commit_message>
reformatted PQ1providedCode to cpp
</commit_message>
<xml_diff>
--- a/OS Unit 3/Unit 3 Slides/SCHED ALG EXAMPLE.xlsx
+++ b/OS Unit 3/Unit 3 Slides/SCHED ALG EXAMPLE.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crincon/Documents/UH/COSC 3360/PPT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laniwang/Desktop/3360_Summer_2023/OS Unit 3/Unit 3 Slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7FE447-1C0B-5C47-9588-7CA4AE8F1180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30860" windowHeight="19640" xr2:uid="{EA549821-EDB0-A64E-8D3E-250BC781A7C6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -90,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -107,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +131,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -138,7 +149,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -149,18 +160,18 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -171,7 +182,7 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -186,7 +197,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -197,7 +208,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -206,27 +217,27 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -234,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -262,6 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,11 +587,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5DA842-6942-8C40-BB3C-06A840F4D86F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AC45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,62 +603,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="21">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="21">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="21">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="21">
         <v>6</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="B4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="21">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21">
         <v>6</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="21">
         <v>4</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="21">
         <v>5</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="21">
         <v>2</v>
       </c>
       <c r="I4">
@@ -655,7 +667,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="H5" t="s">
+      <c r="H5" s="21" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1250,19 +1262,19 @@
         <v>3</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:G21" si="4">D20-D3</f>
+        <f>D20-D3</f>
         <v>7</v>
       </c>
       <c r="E21">
-        <f t="shared" si="4"/>
+        <f>E20-E3</f>
         <v>11</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
+        <f>F20-F3</f>
         <v>14</v>
       </c>
       <c r="G21">
-        <f t="shared" si="4"/>
+        <f>G20-G3</f>
         <v>3</v>
       </c>
       <c r="H21">
@@ -1302,19 +1314,19 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22:G22" si="5">D21/D4</f>
+        <f>D21/D4</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="E22">
-        <f t="shared" si="5"/>
+        <f>E21/E4</f>
         <v>2.75</v>
       </c>
       <c r="F22">
-        <f t="shared" si="5"/>
+        <f>F21/F4</f>
         <v>2.8</v>
       </c>
       <c r="G22">
-        <f t="shared" si="5"/>
+        <f>G21/G4</f>
         <v>1.5</v>
       </c>
       <c r="H22">
@@ -1371,22 +1383,22 @@
       <c r="AC23" s="18"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="B24" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E24" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E24" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="21" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="3" t="s">
@@ -1414,22 +1426,22 @@
       <c r="AC24" s="19"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="B25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="21">
         <v>0</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="21">
         <v>2</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="21">
         <v>4</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="21">
         <v>6</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="21">
         <v>8</v>
       </c>
       <c r="I25" s="1"/>
@@ -1495,45 +1507,45 @@
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="B26" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="21">
+        <v>3</v>
+      </c>
+      <c r="D26" s="21">
         <v>6</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="21">
         <v>4</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="21">
         <v>5</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="21">
         <v>2</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+      <c r="B27" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="18">
+        <v>3</v>
+      </c>
+      <c r="D27" s="18">
         <v>15</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="18">
         <v>8</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="18">
         <v>20</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="18">
         <v>10</v>
       </c>
       <c r="I27" s="2" t="s">
@@ -1554,19 +1566,19 @@
         <v>3</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:G28" si="6">D27-D25</f>
+        <f t="shared" ref="D28:G28" si="4">D27-D25</f>
         <v>13</v>
       </c>
       <c r="E28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="F28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H28">
@@ -1591,19 +1603,19 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29:G29" si="7">D28/D26</f>
+        <f t="shared" ref="D29:G29" si="5">D28/D26</f>
         <v>2.1666666666666665</v>
       </c>
       <c r="E29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>2.8</v>
       </c>
       <c r="G29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H29">
@@ -1756,19 +1768,19 @@
         <v>3</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:G35" si="8">D34-D25</f>
+        <f t="shared" ref="D35:G35" si="6">D34-D25</f>
         <v>7</v>
       </c>
       <c r="E35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="F35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="G35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="H35">
@@ -1793,19 +1805,19 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <f t="shared" ref="D36:G36" si="9">D35/D26</f>
+        <f t="shared" ref="D36:G36" si="7">D35/D26</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="E36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2.25</v>
       </c>
       <c r="F36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2.8</v>
       </c>
       <c r="G36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3.5</v>
       </c>
       <c r="H36">

</xml_diff>